<commit_message>
First version, second trial from GitHub Desktop. without excel
</commit_message>
<xml_diff>
--- a/IBM6540/GenAIIbm/images/SimpleLLMNetwork.xlsx
+++ b/IBM6540/GenAIIbm/images/SimpleLLMNetwork.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CalPoly\EC4990AINew\AIBookSlides\IBM6540\GenAIIbm\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D398C7B9-C5D8-4800-9B06-C7B4C4C26C20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{100C24DD-84CF-4F51-8555-B30E9504F908}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="45" yWindow="-21720" windowWidth="38640" windowHeight="21840" activeTab="4" xr2:uid="{B76931BD-440B-456E-AFB1-6BA9417F1C68}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="47">
   <si>
     <t>Apple</t>
   </si>
@@ -198,15 +198,6 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Eat </t>
-  </si>
-  <si>
-    <t>amazing</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> apples</t>
-  </si>
-  <si>
     <t xml:space="preserve"> =</t>
   </si>
   <si>
@@ -216,10 +207,23 @@
     <t xml:space="preserve">Position-Aware </t>
   </si>
   <si>
-    <t>Vector for Amazing</t>
-  </si>
-  <si>
     <t>Position Vector*</t>
+  </si>
+  <si>
+    <t>Dog</t>
+  </si>
+  <si>
+    <t>bit</t>
+  </si>
+  <si>
+    <t>child</t>
+  </si>
+  <si>
+    <t>Vector for "bit"</t>
+  </si>
+  <si>
+    <t>Embedding:
+ "bit"</t>
   </si>
   <si>
     <r>
@@ -243,7 +247,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>) Reflects position 2 of "Amazing"</t>
+      <t>) Reflects position 2 of  "bit"</t>
     </r>
   </si>
 </sst>
@@ -252,9 +256,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -338,20 +342,38 @@
     </font>
     <font>
       <b/>
-      <sz val="14"/>
-      <color rgb="FFFF0000"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <vertAlign val="superscript"/>
       <sz val="14"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial Black"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Arial Black"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial Black"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -416,24 +438,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -442,11 +446,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -524,6 +554,10 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -536,43 +570,47 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -603,7 +641,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>205740</xdr:colOff>
+      <xdr:colOff>209550</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -701,7 +739,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="2324100" y="590550"/>
+          <a:off x="2266950" y="590550"/>
           <a:ext cx="5638800" cy="5600700"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -735,9 +773,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
+      <xdr:colOff>167640</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>98536</xdr:rowOff>
+      <xdr:rowOff>94726</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1093,7 +1131,7 @@
   <dimension ref="B1:Q15"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1:P13"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1151,14 +1189,14 @@
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>2</v>
+      <c r="C4" s="2">
+        <v>0</v>
       </c>
       <c r="N4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="P4" s="2" t="s">
-        <v>2</v>
+      <c r="P4" s="2">
+        <v>0</v>
       </c>
       <c r="Q4" s="1" t="s">
         <v>2</v>
@@ -1168,14 +1206,14 @@
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>2</v>
+      <c r="C5" s="2">
+        <v>0</v>
       </c>
       <c r="N5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="P5" s="2" t="s">
-        <v>2</v>
+      <c r="P5" s="2">
+        <v>0</v>
       </c>
       <c r="Q5" s="1" t="s">
         <v>2</v>
@@ -1185,14 +1223,14 @@
       <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>2</v>
+      <c r="C6" s="2">
+        <v>0</v>
       </c>
       <c r="N6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="P6" s="2" t="s">
-        <v>2</v>
+      <c r="P6" s="2">
+        <v>0</v>
       </c>
       <c r="Q6" s="1" t="s">
         <v>2</v>
@@ -1202,14 +1240,14 @@
       <c r="B7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>2</v>
+      <c r="C7" s="2">
+        <v>0</v>
       </c>
       <c r="N7" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="P7" s="2" t="s">
-        <v>2</v>
+      <c r="P7" s="2">
+        <v>0</v>
       </c>
       <c r="Q7" s="1" t="s">
         <v>2</v>
@@ -1219,14 +1257,14 @@
       <c r="B8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>2</v>
+      <c r="C8" s="2">
+        <v>0</v>
       </c>
       <c r="N8" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="P8" s="2" t="s">
-        <v>2</v>
+      <c r="P8" s="2">
+        <v>0</v>
       </c>
       <c r="Q8" s="1" t="s">
         <v>2</v>
@@ -1253,14 +1291,14 @@
       <c r="B10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>2</v>
+      <c r="C10" s="2">
+        <v>0</v>
       </c>
       <c r="N10" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="P10" s="2" t="s">
-        <v>2</v>
+      <c r="P10" s="2">
+        <v>0</v>
       </c>
       <c r="Q10" s="1" t="s">
         <v>2</v>
@@ -1287,14 +1325,14 @@
       <c r="B12" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>2</v>
+      <c r="C12" s="2">
+        <v>0</v>
       </c>
       <c r="N12" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="P12" s="2" t="s">
-        <v>2</v>
+      <c r="P12" s="2">
+        <v>0</v>
       </c>
       <c r="Q12" s="1" t="s">
         <v>2</v>
@@ -1345,7 +1383,7 @@
   <dimension ref="B1:Q15"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+      <selection activeCell="Q16" sqref="Q16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1357,7 +1395,9 @@
     <col min="15" max="15" width="2.88671875" style="1" customWidth="1"/>
     <col min="16" max="16" width="12.109375" style="1" customWidth="1"/>
     <col min="17" max="17" width="12.21875" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="8.88671875" style="1"/>
+    <col min="18" max="31" width="8.88671875" style="1"/>
+    <col min="32" max="32" width="8.88671875" style="1" customWidth="1"/>
+    <col min="33" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:17" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
@@ -1403,14 +1443,14 @@
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>2</v>
+      <c r="C4" s="2">
+        <v>0</v>
       </c>
       <c r="N4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="P4" s="2" t="s">
-        <v>2</v>
+      <c r="P4" s="2">
+        <v>0</v>
       </c>
       <c r="Q4" s="1" t="s">
         <v>2</v>
@@ -1420,14 +1460,14 @@
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>2</v>
+      <c r="C5" s="2">
+        <v>0</v>
       </c>
       <c r="N5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="P5" s="2" t="s">
-        <v>2</v>
+      <c r="P5" s="2">
+        <v>0</v>
       </c>
       <c r="Q5" s="1" t="s">
         <v>2</v>
@@ -1437,14 +1477,14 @@
       <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>2</v>
+      <c r="C6" s="2">
+        <v>0</v>
       </c>
       <c r="N6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="P6" s="2" t="s">
-        <v>2</v>
+      <c r="P6" s="2">
+        <v>0</v>
       </c>
       <c r="Q6" s="1" t="s">
         <v>2</v>
@@ -1454,14 +1494,14 @@
       <c r="B7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>2</v>
+      <c r="C7" s="2">
+        <v>0</v>
       </c>
       <c r="N7" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="P7" s="2" t="s">
-        <v>2</v>
+      <c r="P7" s="2">
+        <v>0</v>
       </c>
       <c r="Q7" s="1" t="s">
         <v>2</v>
@@ -1471,14 +1511,14 @@
       <c r="B8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>2</v>
+      <c r="C8" s="2">
+        <v>0</v>
       </c>
       <c r="N8" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="P8" s="2" t="s">
-        <v>2</v>
+      <c r="P8" s="2">
+        <v>0</v>
       </c>
       <c r="Q8" s="1" t="s">
         <v>2</v>
@@ -1505,14 +1545,14 @@
       <c r="B10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>2</v>
+      <c r="C10" s="2">
+        <v>0</v>
       </c>
       <c r="N10" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="P10" s="2" t="s">
-        <v>2</v>
+      <c r="P10" s="2">
+        <v>0</v>
       </c>
       <c r="Q10" s="1" t="s">
         <v>2</v>
@@ -1539,14 +1579,14 @@
       <c r="B12" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>2</v>
+      <c r="C12" s="2">
+        <v>0</v>
       </c>
       <c r="N12" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="P12" s="2" t="s">
-        <v>2</v>
+      <c r="P12" s="2">
+        <v>0</v>
       </c>
       <c r="Q12" s="1" t="s">
         <v>2</v>
@@ -2636,7 +2676,7 @@
   <dimension ref="B2:Y17"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2675,10 +2715,10 @@
       <c r="M2" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="Q2" s="27" t="s">
+      <c r="Q2" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="R2" s="27"/>
+      <c r="R2" s="29"/>
       <c r="V2" s="26" t="s">
         <v>8</v>
       </c>
@@ -2709,20 +2749,20 @@
       <c r="B4" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="28" t="s">
+      <c r="D4" s="30" t="s">
         <v>35</v>
       </c>
       <c r="E4" s="12">
         <v>0</v>
       </c>
-      <c r="G4" s="29" t="s">
+      <c r="G4" s="31" t="s">
         <v>34</v>
       </c>
       <c r="H4" s="18">
         <v>0</v>
       </c>
       <c r="I4" s="14"/>
-      <c r="J4" s="30" t="s">
+      <c r="J4" s="32" t="s">
         <v>36</v>
       </c>
       <c r="K4" s="21">
@@ -2739,16 +2779,16 @@
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="28"/>
+      <c r="D5" s="30"/>
       <c r="E5" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="29"/>
+      <c r="G5" s="31"/>
       <c r="H5" s="18" t="s">
         <v>2</v>
       </c>
       <c r="I5" s="14"/>
-      <c r="J5" s="30"/>
+      <c r="J5" s="32"/>
       <c r="K5" s="21" t="s">
         <v>2</v>
       </c>
@@ -2763,18 +2803,18 @@
       <c r="B6" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="28"/>
+      <c r="D6" s="30"/>
       <c r="E6" s="12">
-        <v>0</v>
-      </c>
-      <c r="G6" s="29"/>
+        <v>1</v>
+      </c>
+      <c r="G6" s="31"/>
       <c r="H6" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I6" s="14"/>
-      <c r="J6" s="30"/>
+      <c r="J6" s="32"/>
       <c r="K6" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X6" s="24">
         <v>1</v>
@@ -2787,16 +2827,16 @@
       <c r="B7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="28"/>
+      <c r="D7" s="30"/>
       <c r="E7" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G7" s="29"/>
+      <c r="G7" s="31"/>
       <c r="H7" s="18" t="s">
         <v>2</v>
       </c>
       <c r="I7" s="14"/>
-      <c r="J7" s="30"/>
+      <c r="J7" s="32"/>
       <c r="K7" s="21" t="s">
         <v>2</v>
       </c>
@@ -2809,16 +2849,16 @@
       <c r="B8" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="28"/>
+      <c r="D8" s="30"/>
       <c r="E8" s="12">
         <v>1</v>
       </c>
-      <c r="G8" s="29"/>
+      <c r="G8" s="31"/>
       <c r="H8" s="18">
         <v>0</v>
       </c>
       <c r="I8" s="14"/>
-      <c r="J8" s="30"/>
+      <c r="J8" s="32"/>
       <c r="K8" s="21">
         <v>0</v>
       </c>
@@ -2833,16 +2873,16 @@
       <c r="B9" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="28"/>
+      <c r="D9" s="30"/>
       <c r="E9" s="12">
         <v>1</v>
       </c>
-      <c r="G9" s="29"/>
+      <c r="G9" s="31"/>
       <c r="H9" s="18">
         <v>0</v>
       </c>
       <c r="I9" s="14"/>
-      <c r="J9" s="30"/>
+      <c r="J9" s="32"/>
       <c r="K9" s="21">
         <v>0</v>
       </c>
@@ -2857,16 +2897,16 @@
       <c r="B10" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="28"/>
+      <c r="D10" s="30"/>
       <c r="E10" s="12">
         <v>0</v>
       </c>
-      <c r="G10" s="29"/>
+      <c r="G10" s="31"/>
       <c r="H10" s="18">
         <v>0</v>
       </c>
       <c r="I10" s="14"/>
-      <c r="J10" s="30"/>
+      <c r="J10" s="32"/>
       <c r="K10" s="21">
         <v>1</v>
       </c>
@@ -2881,16 +2921,16 @@
       <c r="B11" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="28"/>
+      <c r="D11" s="30"/>
       <c r="E11" s="12">
         <v>0</v>
       </c>
-      <c r="G11" s="29"/>
+      <c r="G11" s="31"/>
       <c r="H11" s="18">
         <v>1</v>
       </c>
       <c r="I11" s="14"/>
-      <c r="J11" s="30"/>
+      <c r="J11" s="32"/>
       <c r="K11" s="21">
         <v>0</v>
       </c>
@@ -2905,16 +2945,16 @@
       <c r="B12" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D12" s="28"/>
+      <c r="D12" s="30"/>
       <c r="E12" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G12" s="29"/>
+      <c r="G12" s="31"/>
       <c r="H12" s="18" t="s">
         <v>2</v>
       </c>
       <c r="I12" s="14"/>
-      <c r="J12" s="30"/>
+      <c r="J12" s="32"/>
       <c r="K12" s="21" t="s">
         <v>2</v>
       </c>
@@ -2929,16 +2969,16 @@
       <c r="B13" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="28"/>
+      <c r="D13" s="30"/>
       <c r="E13" s="12">
         <v>0</v>
       </c>
-      <c r="G13" s="29"/>
+      <c r="G13" s="31"/>
       <c r="H13" s="18">
         <v>1</v>
       </c>
       <c r="I13" s="14"/>
-      <c r="J13" s="30"/>
+      <c r="J13" s="32"/>
       <c r="K13" s="21">
         <v>0</v>
       </c>
@@ -2953,16 +2993,16 @@
       <c r="B14" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D14" s="28"/>
+      <c r="D14" s="30"/>
       <c r="E14" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G14" s="29"/>
+      <c r="G14" s="31"/>
       <c r="H14" s="18" t="s">
         <v>2</v>
       </c>
       <c r="I14" s="14"/>
-      <c r="J14" s="30"/>
+      <c r="J14" s="32"/>
       <c r="K14" s="21" t="s">
         <v>2</v>
       </c>
@@ -3029,68 +3069,70 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1B33766-D588-4ED0-83DA-6692DFF32000}">
-  <dimension ref="D2:K25"/>
+  <dimension ref="D1:K29"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="14.33203125" customWidth="1"/>
+    <col min="3" max="3" width="5.109375" customWidth="1"/>
+    <col min="4" max="4" width="16.88671875" customWidth="1"/>
     <col min="5" max="5" width="10.77734375" customWidth="1"/>
     <col min="7" max="7" width="12.33203125" customWidth="1"/>
     <col min="8" max="8" width="11.5546875" customWidth="1"/>
     <col min="9" max="9" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:11" ht="18" x14ac:dyDescent="0.3">
-      <c r="D2" s="42">
+    <row r="1" spans="4:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="4:11" ht="21" x14ac:dyDescent="0.3">
+      <c r="D2" s="43">
         <v>1</v>
       </c>
-      <c r="E2" s="43">
+      <c r="E2" s="44">
         <v>2</v>
       </c>
       <c r="F2" s="43">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="4:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="D3" s="44" t="s">
-        <v>37</v>
-      </c>
-      <c r="E3" s="39" t="s">
-        <v>38</v>
-      </c>
-      <c r="F3" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="G3" s="31"/>
-      <c r="H3" s="31"/>
+    <row r="3" spans="4:11" ht="21.6" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="D3" s="45" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" s="46" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" s="47" t="s">
+        <v>43</v>
+      </c>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
     </row>
     <row r="4" spans="4:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
     </row>
     <row r="5" spans="4:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="31"/>
-      <c r="H5" s="31"/>
-    </row>
-    <row r="6" spans="4:11" ht="21" x14ac:dyDescent="0.35">
-      <c r="D6" s="32" t="s">
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="27"/>
+    </row>
+    <row r="6" spans="4:11" ht="18.600000000000001" x14ac:dyDescent="0.3">
+      <c r="D6" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="32"/>
-      <c r="F6" s="32" t="s">
+      <c r="E6" s="33"/>
+      <c r="F6" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="31"/>
+      <c r="G6" s="34"/>
       <c r="H6" s="35" t="s">
         <v>11</v>
       </c>
@@ -3098,254 +3140,256 @@
       <c r="J6" s="35"/>
     </row>
     <row r="7" spans="4:11" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D7" s="35" t="s">
-        <v>19</v>
+      <c r="D7" s="39" t="s">
+        <v>45</v>
       </c>
       <c r="E7" s="35" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F7" s="35"/>
       <c r="G7" s="35"/>
       <c r="H7" s="35" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="I7" s="35"/>
       <c r="J7" s="35"/>
-      <c r="K7" s="40"/>
+      <c r="K7" s="28"/>
     </row>
     <row r="8" spans="4:11" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D8" s="41"/>
+      <c r="D8" s="36"/>
       <c r="E8" s="35"/>
       <c r="F8" s="35"/>
       <c r="G8" s="35"/>
       <c r="H8" s="35" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I8" s="35"/>
       <c r="J8" s="35"/>
     </row>
-    <row r="9" spans="4:11" ht="21" x14ac:dyDescent="0.35">
-      <c r="D9" s="33">
+    <row r="9" spans="4:11" ht="18.600000000000001" x14ac:dyDescent="0.3">
+      <c r="D9" s="37">
         <v>0.03</v>
       </c>
-      <c r="E9" s="32"/>
-      <c r="F9" s="33">
+      <c r="E9" s="33"/>
+      <c r="F9" s="37">
         <v>0.23</v>
       </c>
-      <c r="G9" s="31"/>
-      <c r="H9" s="32"/>
+      <c r="G9" s="34"/>
+      <c r="H9" s="33"/>
       <c r="I9" s="38">
         <f>D9+F9</f>
         <v>0.26</v>
       </c>
-      <c r="J9" s="31"/>
-    </row>
-    <row r="10" spans="4:11" ht="21" x14ac:dyDescent="0.35">
-      <c r="D10" s="33" t="s">
-        <v>2</v>
-      </c>
-      <c r="E10" s="32"/>
-      <c r="F10" s="33" t="s">
-        <v>2</v>
-      </c>
-      <c r="G10" s="31"/>
-      <c r="H10" s="32"/>
-      <c r="I10" s="33" t="s">
-        <v>2</v>
-      </c>
-      <c r="J10" s="31"/>
-    </row>
-    <row r="11" spans="4:11" ht="21" x14ac:dyDescent="0.35">
-      <c r="D11" s="33" t="s">
-        <v>2</v>
-      </c>
-      <c r="E11" s="32"/>
-      <c r="F11" s="33" t="s">
-        <v>2</v>
-      </c>
-      <c r="G11" s="31"/>
-      <c r="H11" s="32"/>
-      <c r="I11" s="33" t="s">
-        <v>2</v>
-      </c>
-      <c r="J11" s="31"/>
-    </row>
-    <row r="12" spans="4:11" ht="21" x14ac:dyDescent="0.35">
-      <c r="D12" s="33" t="s">
-        <v>2</v>
-      </c>
-      <c r="E12" s="32"/>
-      <c r="F12" s="33" t="s">
-        <v>2</v>
-      </c>
-      <c r="G12" s="31"/>
-      <c r="H12" s="32"/>
-      <c r="I12" s="33" t="s">
-        <v>2</v>
-      </c>
-      <c r="J12" s="31"/>
-    </row>
-    <row r="13" spans="4:11" ht="21" x14ac:dyDescent="0.35">
-      <c r="D13" s="33" t="s">
-        <v>2</v>
-      </c>
-      <c r="E13" s="32"/>
-      <c r="F13" s="33" t="s">
-        <v>2</v>
-      </c>
-      <c r="G13" s="31"/>
-      <c r="H13" s="32"/>
-      <c r="I13" s="33" t="s">
-        <v>2</v>
-      </c>
-      <c r="J13" s="31"/>
-    </row>
-    <row r="14" spans="4:11" ht="21" x14ac:dyDescent="0.35">
-      <c r="D14" s="33" t="s">
-        <v>2</v>
-      </c>
-      <c r="E14" s="32" t="s">
-        <v>41</v>
-      </c>
-      <c r="F14" s="33" t="s">
-        <v>2</v>
-      </c>
-      <c r="G14" s="36" t="s">
-        <v>40</v>
-      </c>
-      <c r="H14" s="37"/>
-      <c r="I14" s="33" t="s">
-        <v>2</v>
-      </c>
-      <c r="J14" s="31"/>
-    </row>
-    <row r="15" spans="4:11" ht="21" x14ac:dyDescent="0.35">
-      <c r="D15" s="33">
+      <c r="J9" s="34"/>
+    </row>
+    <row r="10" spans="4:11" ht="18.600000000000001" x14ac:dyDescent="0.3">
+      <c r="D10" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="33"/>
+      <c r="F10" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="G10" s="34"/>
+      <c r="H10" s="33"/>
+      <c r="I10" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="J10" s="34"/>
+    </row>
+    <row r="11" spans="4:11" ht="18.600000000000001" x14ac:dyDescent="0.3">
+      <c r="D11" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="33"/>
+      <c r="F11" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="G11" s="34"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="J11" s="34"/>
+    </row>
+    <row r="12" spans="4:11" ht="18.600000000000001" x14ac:dyDescent="0.3">
+      <c r="D12" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" s="33"/>
+      <c r="F12" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="G12" s="34"/>
+      <c r="H12" s="33"/>
+      <c r="I12" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="J12" s="34"/>
+    </row>
+    <row r="13" spans="4:11" ht="18.600000000000001" x14ac:dyDescent="0.3">
+      <c r="D13" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="33"/>
+      <c r="F13" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="G13" s="34"/>
+      <c r="H13" s="33"/>
+      <c r="I13" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="J13" s="34"/>
+    </row>
+    <row r="14" spans="4:11" ht="25.2" x14ac:dyDescent="0.3">
+      <c r="D14" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14" s="41" t="s">
+        <v>38</v>
+      </c>
+      <c r="F14" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="G14" s="42" t="s">
+        <v>37</v>
+      </c>
+      <c r="H14" s="41"/>
+      <c r="I14" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="J14" s="34"/>
+    </row>
+    <row r="15" spans="4:11" ht="18.600000000000001" x14ac:dyDescent="0.3">
+      <c r="D15" s="37">
         <v>1.2E-2</v>
       </c>
-      <c r="E15" s="32"/>
-      <c r="F15" s="33">
+      <c r="E15" s="33"/>
+      <c r="F15" s="37">
         <v>-0.12</v>
       </c>
-      <c r="G15" s="31"/>
-      <c r="H15" s="32"/>
-      <c r="I15" s="33">
+      <c r="G15" s="34"/>
+      <c r="H15" s="33"/>
+      <c r="I15" s="37">
         <f>D15+F15</f>
         <v>-0.108</v>
       </c>
-      <c r="J15" s="31"/>
-    </row>
-    <row r="16" spans="4:11" ht="21" x14ac:dyDescent="0.35">
-      <c r="D16" s="33" t="s">
-        <v>2</v>
-      </c>
-      <c r="E16" s="32"/>
-      <c r="F16" s="33" t="s">
-        <v>2</v>
-      </c>
-      <c r="G16" s="31"/>
-      <c r="H16" s="32"/>
-      <c r="I16" s="33" t="s">
-        <v>2</v>
-      </c>
-      <c r="J16" s="31"/>
-    </row>
-    <row r="17" spans="4:10" ht="21" x14ac:dyDescent="0.35">
-      <c r="D17" s="33">
+      <c r="J15" s="34"/>
+    </row>
+    <row r="16" spans="4:11" ht="18.600000000000001" x14ac:dyDescent="0.3">
+      <c r="D16" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="E16" s="33"/>
+      <c r="F16" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="G16" s="34"/>
+      <c r="H16" s="33"/>
+      <c r="I16" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="J16" s="34"/>
+    </row>
+    <row r="17" spans="4:10" ht="18.600000000000001" x14ac:dyDescent="0.3">
+      <c r="D17" s="37">
         <v>2E-3</v>
       </c>
-      <c r="E17" s="32"/>
-      <c r="F17" s="33">
+      <c r="E17" s="33"/>
+      <c r="F17" s="37">
         <v>0.75</v>
       </c>
-      <c r="G17" s="31"/>
-      <c r="H17" s="32"/>
-      <c r="I17" s="33">
+      <c r="G17" s="34"/>
+      <c r="H17" s="33"/>
+      <c r="I17" s="37">
         <f>D17+F17</f>
         <v>0.752</v>
       </c>
-      <c r="J17" s="31"/>
-    </row>
-    <row r="18" spans="4:10" ht="21" x14ac:dyDescent="0.35">
-      <c r="D18" s="33" t="s">
-        <v>2</v>
-      </c>
-      <c r="E18" s="32"/>
-      <c r="F18" s="33" t="s">
-        <v>2</v>
-      </c>
-      <c r="G18" s="31"/>
-      <c r="H18" s="32"/>
-      <c r="I18" s="33" t="s">
-        <v>2</v>
-      </c>
-      <c r="J18" s="31"/>
-    </row>
-    <row r="19" spans="4:10" ht="21" x14ac:dyDescent="0.35">
-      <c r="D19" s="33">
+      <c r="J17" s="34"/>
+    </row>
+    <row r="18" spans="4:10" ht="18.600000000000001" x14ac:dyDescent="0.3">
+      <c r="D18" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="E18" s="33"/>
+      <c r="F18" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="G18" s="34"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="J18" s="34"/>
+    </row>
+    <row r="19" spans="4:10" ht="18.600000000000001" x14ac:dyDescent="0.3">
+      <c r="D19" s="37">
         <v>0.01</v>
       </c>
-      <c r="E19" s="32"/>
-      <c r="F19" s="33">
+      <c r="E19" s="33"/>
+      <c r="F19" s="37">
         <v>0.01</v>
       </c>
-      <c r="G19" s="31"/>
-      <c r="H19" s="32"/>
-      <c r="I19" s="33">
+      <c r="G19" s="34"/>
+      <c r="H19" s="33"/>
+      <c r="I19" s="37">
         <f>D19+F19</f>
         <v>0.02</v>
       </c>
-      <c r="J19" s="31"/>
+      <c r="J19" s="34"/>
     </row>
     <row r="20" spans="4:10" ht="18" x14ac:dyDescent="0.35">
-      <c r="D20" s="31"/>
-      <c r="E20" s="31"/>
-      <c r="F20" s="31"/>
-      <c r="G20" s="31"/>
-      <c r="H20" s="31"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="27"/>
     </row>
     <row r="21" spans="4:10" ht="19.8" x14ac:dyDescent="0.35">
-      <c r="D21" s="34" t="s">
-        <v>45</v>
-      </c>
-      <c r="E21" s="31"/>
-      <c r="F21" s="31"/>
-      <c r="G21" s="31"/>
-      <c r="H21" s="31"/>
+      <c r="D21" s="40" t="s">
+        <v>46</v>
+      </c>
+      <c r="E21" s="27"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="27"/>
+      <c r="H21" s="27"/>
     </row>
     <row r="22" spans="4:10" ht="18" x14ac:dyDescent="0.35">
-      <c r="D22" s="31"/>
-      <c r="E22" s="31"/>
-      <c r="F22" s="31"/>
-      <c r="G22" s="31"/>
-      <c r="H22" s="31"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="27"/>
+      <c r="F22" s="27"/>
+      <c r="G22" s="27"/>
+      <c r="H22" s="27"/>
     </row>
     <row r="23" spans="4:10" ht="18" x14ac:dyDescent="0.35">
-      <c r="D23" s="31"/>
-      <c r="E23" s="31"/>
-      <c r="F23" s="31"/>
-      <c r="G23" s="31"/>
-      <c r="H23" s="31"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="27"/>
+      <c r="F23" s="27"/>
+      <c r="G23" s="27"/>
+      <c r="H23" s="27"/>
     </row>
     <row r="24" spans="4:10" ht="18" x14ac:dyDescent="0.35">
-      <c r="D24" s="31"/>
-      <c r="E24" s="31"/>
-      <c r="F24" s="31"/>
-      <c r="G24" s="31"/>
-      <c r="H24" s="31"/>
+      <c r="D24" s="27"/>
+      <c r="E24" s="27"/>
+      <c r="F24" s="27"/>
+      <c r="G24" s="27"/>
+      <c r="H24" s="27"/>
     </row>
     <row r="25" spans="4:10" ht="18" x14ac:dyDescent="0.35">
-      <c r="D25" s="31"/>
-      <c r="E25" s="31"/>
-      <c r="F25" s="31"/>
-      <c r="G25" s="31"/>
-      <c r="H25" s="31"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="27"/>
+      <c r="F25" s="27"/>
+      <c r="G25" s="27"/>
+      <c r="H25" s="27"/>
+    </row>
+    <row r="29" spans="4:10" ht="25.2" x14ac:dyDescent="0.3">
+      <c r="G29" s="41"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="5">
     <mergeCell ref="D7:D8"/>
     <mergeCell ref="E7:G8"/>
-    <mergeCell ref="G14:H14"/>
     <mergeCell ref="H6:J6"/>
     <mergeCell ref="H8:J8"/>
     <mergeCell ref="H7:J7"/>

</xml_diff>